<commit_message>
improved random forest model (dog-to-human)
</commit_message>
<xml_diff>
--- a/FILE-DATA_DICTIONARY.xlsx
+++ b/FILE-DATA_DICTIONARY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romina\Desktop\HW reposistories\Group-Project-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D93CD76-3F7C-421C-BA7B-606A33C72E12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A3B01D-A5B9-492D-8AB5-B28C3108027E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36" yWindow="0" windowWidth="9300" windowHeight="12360" firstSheet="1" activeTab="1" xr2:uid="{66A37A70-FEF1-4D24-B201-6D02ECA5CECC}"/>
+    <workbookView xWindow="4272" yWindow="72" windowWidth="12372" windowHeight="12564" activeTab="1" xr2:uid="{66A37A70-FEF1-4D24-B201-6D02ECA5CECC}"/>
   </bookViews>
   <sheets>
     <sheet name="file_description" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="136">
   <si>
     <t>metadata_otu_merged.csv</t>
   </si>
@@ -428,6 +428,18 @@
   </si>
   <si>
     <t>ro</t>
+  </si>
+  <si>
+    <t>transposed_OTU</t>
+  </si>
+  <si>
+    <t>metadata_otu_merged_non-rarefied</t>
+  </si>
+  <si>
+    <t>original out_table, transposed (non-rarefied)</t>
+  </si>
+  <si>
+    <t>transposed_OTU merged with metadata</t>
   </si>
 </sst>
 </file>
@@ -471,7 +483,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -507,24 +519,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -535,7 +534,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -868,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542C1445-450D-408D-B856-758E95C4D7BE}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,6 +960,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -970,696 +990,642 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44BFB23E-D563-4D89-9D83-F0E9DFF00FE3}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="28.21875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="24.77734375" style="12" customWidth="1"/>
-    <col min="6" max="6" width="16" style="8" customWidth="1"/>
+    <col min="3" max="3" width="28.21875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="D26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="D27" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="D28" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="D30" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="D31" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="D32" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="D33" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="D34" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="D35" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="D36" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="D37" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="11" t="s">
+      <c r="C38" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="D38" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F38" s="7"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="11" t="s">
+      <c r="C39" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="D39" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F39" s="7"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="11" t="s">
+      <c r="C40" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="D40" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F40" s="7"/>
-      <c r="J40" t="s">
+      <c r="E40" s="6"/>
+      <c r="I40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="D41" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="D42" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F42" s="7"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="11" t="s">
+      <c r="C43" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="D43" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="F43" s="7"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="11" t="s">
+      <c r="C44" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="D44" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="F44" s="7"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="D45" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F45" s="7"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="11" t="s">
+      <c r="C46" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="D46" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="F46" s="7"/>
-    </row>
-    <row r="47" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="11" t="s">
+      <c r="C47" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="D47" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F47" s="7"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="11" t="s">
+      <c r="C48" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="D48" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="F48" s="7"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="11" t="s">
+      <c r="C49" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="D49" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="F49" s="7"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="11" t="s">
+      <c r="C50" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="D50" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F50" s="7"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="D51" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F51" s="7"/>
+      <c r="E51" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>